<commit_message>
changing logic of headers support
</commit_message>
<xml_diff>
--- a/python/tests/fixtures/fixture-changing-header-location.xlsx
+++ b/python/tests/fixtures/fixture-changing-header-location.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="January" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Values" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
   <si>
     <t xml:space="preserve">Years Sheet</t>
   </si>
@@ -158,15 +159,15 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B21" activeCellId="1" sqref="A12:B14 B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.85"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="256" min="3" style="1" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="256" min="3" style="1" width="10.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -218,10 +219,10 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="1" sqref="A12:B14 D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
@@ -243,6 +244,75 @@
       </c>
       <c r="C2" s="0" t="n">
         <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12:B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="256" min="3" style="1" width="10.85"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0"/>
+      <c r="B2" s="0"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0"/>
+      <c r="B3" s="0"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0"/>
+      <c r="B4" s="0"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B13" s="4" t="n">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1" t="n">
+        <v>2020</v>
       </c>
     </row>
   </sheetData>

</xml_diff>